<commit_message>
Changes to attendance list, removal of old files
</commit_message>
<xml_diff>
--- a/FA17/MA122/AttendanceSheet003.xlsx
+++ b/FA17/MA122/AttendanceSheet003.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="135">
   <si>
     <t>Arrain</t>
   </si>
@@ -85,12 +85,6 @@
   </si>
   <si>
     <t>RYAN</t>
-  </si>
-  <si>
-    <t>Cheng</t>
-  </si>
-  <si>
-    <t>VIVIAN</t>
   </si>
   <si>
     <t>Colter</t>
@@ -1245,7 +1239,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1256,10 +1250,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O71"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1671,10 +1665,10 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1692,10 +1686,10 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="1" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>115</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1713,10 +1707,10 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>132</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>133</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1734,10 +1728,10 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="1" t="s">
-        <v>134</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1902,10 +1896,10 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1923,10 +1917,10 @@
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="1" t="s">
-        <v>116</v>
+        <v>52</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2091,10 +2085,10 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="1" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2112,10 +2106,10 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="1" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2280,10 +2274,10 @@
     </row>
     <row r="48" spans="1:15">
       <c r="A48" s="1" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2322,10 +2316,10 @@
     </row>
     <row r="50" spans="1:15">
       <c r="A50" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>123</v>
+        <v>84</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2343,10 +2337,10 @@
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="1" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2364,10 +2358,10 @@
     </row>
     <row r="52" spans="1:15">
       <c r="A52" s="1" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>125</v>
+        <v>31</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -2385,10 +2379,10 @@
     </row>
     <row r="53" spans="1:15">
       <c r="A53" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -2553,10 +2547,10 @@
     </row>
     <row r="61" spans="1:15">
       <c r="A61" s="1" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -2574,10 +2568,10 @@
     </row>
     <row r="62" spans="1:15">
       <c r="A62" s="1" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -2619,7 +2613,7 @@
         <v>106</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2637,10 +2631,10 @@
     </row>
     <row r="65" spans="1:15">
       <c r="A65" s="1" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -2658,10 +2652,10 @@
     </row>
     <row r="66" spans="1:15">
       <c r="A66" s="1" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -2682,7 +2676,7 @@
         <v>109</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>110</v>
+        <v>17</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2700,10 +2694,10 @@
     </row>
     <row r="68" spans="1:15">
       <c r="A68" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2721,10 +2715,10 @@
     </row>
     <row r="69" spans="1:15">
       <c r="A69" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2761,27 +2755,6 @@
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
     </row>
-    <row r="71" spans="1:15">
-      <c r="A71" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-    </row>
   </sheetData>
   <sortState ref="A1:B71">
     <sortCondition ref="A31"/>

</xml_diff>